<commit_message>
Added User Registration with Different Email Verification Flows
</commit_message>
<xml_diff>
--- a/TestCases_of_Idx-Auto-Tester.xlsx
+++ b/TestCases_of_Idx-Auto-Tester.xlsx
@@ -88,11 +88,13 @@
     <t>Verify that user is able to register with valid data</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Navigate to Site URL
+    <t>1. Navigate to Site URL
 2. Check that Login button displaying on page
 3. Click on Create Account link displaying on page
 4. Enter Email Id, Password, Confirm Password and other displayed fields
-5. Click on Register button </t>
+5. Click on Register button 
+6. Verify notification message displayed on page if email verification is required
+7. If email verification is optional/disabled then check profile page and logout from application</t>
   </si>
   <si>
     <t>User should able to register with entered data and notification message should display for verification of email.</t>
@@ -101,15 +103,17 @@
     <t>TC_05</t>
   </si>
   <si>
-    <t>Verify that user is able to verify email for registered user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Navigate to Site URL
+    <t>Verify that user is able to verify email for registered user if email verification flow is required</t>
+  </si>
+  <si>
+    <t>1. Navigate to Site URL
+2. Check email verification flow is required or not
 2. Check verification email to above registered email id 
-3. Click on verification link or copy paste on link on browser </t>
-  </si>
-  <si>
-    <t>User should able to verify received verification email successfully.</t>
+3. Click on verification link or copy paste on link on browser 
+4. If email verification flow is optional or disabled then assert message</t>
+  </si>
+  <si>
+    <t>User should able to verify received verification email successfully with required email verification flow.</t>
   </si>
   <si>
     <t>TC_06</t>
@@ -987,7 +991,7 @@
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="3"/>
@@ -1019,14 +1023,14 @@
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="3"/>

</xml_diff>

<commit_message>
Updated test cases sheet
</commit_message>
<xml_diff>
--- a/TestCases_of_Idx-Auto-Tester.xlsx
+++ b/TestCases_of_Idx-Auto-Tester.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miITF5WLBxD+qvt9+tBHsY2dnb8qg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi56KB2OgTyHqhRR8VC/H+sOOcirA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t>Test case ID</t>
   </si>
@@ -358,10 +358,30 @@
     <t>User should receive error message of 'The Confirm Password field does not match the Password field.'</t>
   </si>
   <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>Verify that user should unable to change password with new password same as current password</t>
+  </si>
+  <si>
+    <t>1. Create user by account api with sample payload using loginradius-sdk 
+2. Navigate to Site URL
+3. Navigate to Login Page
+4. Enter Email Id and Password which used in sample payload
+5. Click on Login button 
+6. Check that navigated to profile page
+7. Navigate to Account Menu &gt; Change Password
+8. Enter valid Current Password in Old Password, New Password, Confirm Password
+9. Click on Submit button</t>
+  </si>
+  <si>
+    <t>User should receive error message of 'Your new password is too similar to your old passwords, please try a different password.'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Cases of Profile Editor Feature </t>
   </si>
   <si>
-    <t>TC_20</t>
+    <t>TC_21</t>
   </si>
   <si>
     <t>Verify that user is able to update profile after logged-in</t>
@@ -382,7 +402,7 @@
     <t>User should able to update profile successfully with new data.</t>
   </si>
   <si>
-    <t>TC_21</t>
+    <t>TC_22</t>
   </si>
   <si>
     <t>Verify that user is able to update profile with blank last name field</t>
@@ -405,7 +425,7 @@
     <t xml:space="preserve">Test Cases of Forgot Password Feature </t>
   </si>
   <si>
-    <t>TC_22</t>
+    <t>TC_23</t>
   </si>
   <si>
     <t>Verify that user is able to reset password by using forgot password option</t>
@@ -430,7 +450,7 @@
     <t xml:space="preserve">Test Cases of Passwordless Login Feature </t>
   </si>
   <si>
-    <t>TC_23</t>
+    <t>TC_24</t>
   </si>
   <si>
     <t>Verify that user is able to login by passwordless login using email</t>
@@ -452,7 +472,7 @@
     <t>User should able to login successfully with passwordless login using email feature.</t>
   </si>
   <si>
-    <t>TC_24</t>
+    <t>TC_25</t>
   </si>
   <si>
     <t>Verify that application sends the login link when login by unverified user's email</t>
@@ -471,7 +491,7 @@
     <t>User should receive verification link when try to login with unverified email.</t>
   </si>
   <si>
-    <t>TC_25</t>
+    <t>TC_26</t>
   </si>
   <si>
     <t>Verify that application is displaying validation message when pass email in invalid format</t>
@@ -486,6 +506,57 @@
   </si>
   <si>
     <t>User should get validation message on entering invalid email id for login.</t>
+  </si>
+  <si>
+    <t>Test Cases of ForgotPassword by Phone</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>Verify that user is able to perform forgot password journey with valid registered phone number</t>
+  </si>
+  <si>
+    <t>1. Create user by account api with sample payload using loginradius-sdk 
+2. Navigate to Site URL
+3. Navigate to Forgot Password Page
+4. Enter registered Phone number which used in sample payload
+5. Click on Send button 
+6. Check that notification message displaying for further instruction send to provided phone number</t>
+  </si>
+  <si>
+    <t>User should able to perform forgot password journey</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to perform forgot password journey with not registered phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to Site URL
+2. Navigate to Forgot Password Page
+3. Enter not registered Phone number
+4. Click on Send button 
+</t>
+  </si>
+  <si>
+    <t>User should get error message for not registered phone number</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to perform forgot password journey with empty phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to Site URL
+2. Navigate to Forgot Password Page
+3. Click on Send button 
+</t>
+  </si>
+  <si>
+    <t>User should get error message for empty phone number</t>
   </si>
 </sst>
 </file>
@@ -549,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -568,12 +639,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -588,13 +653,22 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,14 +992,14 @@
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="3"/>
@@ -991,7 +1065,7 @@
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="3"/>
@@ -1023,14 +1097,14 @@
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="3"/>
@@ -1293,7 +1367,7 @@
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1328,7 +1402,7 @@
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1553,111 +1627,112 @@
       <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="12"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="10"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="12"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="10"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D25" s="8"/>
+      <c r="E25" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="5" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="10"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>88</v>
       </c>
       <c r="F26" s="3"/>
@@ -1682,7 +1757,7 @@
       <c r="Y26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1716,9 +1791,19 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
+    <row r="28">
+      <c r="A28" s="11" t="s">
         <v>93</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1741,18 +1826,8 @@
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
     </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="5" t="s">
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="4" t="s">
         <v>97</v>
       </c>
       <c r="F29" s="3"/>
@@ -1776,9 +1851,19 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="14" t="s">
+    <row r="30">
+      <c r="A30" s="11" t="s">
         <v>98</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1801,18 +1886,8 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
     </row>
-    <row r="31">
-      <c r="A31" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="6" t="s">
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="4" t="s">
         <v>102</v>
       </c>
       <c r="F31" s="3"/>
@@ -1837,17 +1912,17 @@
       <c r="Y31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>105</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
         <v>106</v>
       </c>
       <c r="F32" s="3"/>
@@ -1872,17 +1947,17 @@
       <c r="Y32" s="3"/>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="5" t="s">
         <v>110</v>
       </c>
       <c r="F33" s="3"/>
@@ -1906,12 +1981,20 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+    <row r="34">
+      <c r="A34" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="D34" s="3"/>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -1934,11 +2017,9 @@
       <c r="Y34" s="3"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="5"/>
+      <c r="A35" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1960,12 +2041,20 @@
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+    <row r="36" ht="99.75" customHeight="1">
+      <c r="A36" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>118</v>
+      </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="5"/>
+      <c r="E36" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1987,12 +2076,20 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+    <row r="37" ht="49.5" customHeight="1">
+      <c r="A37" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="5"/>
+      <c r="E37" s="15" t="s">
+        <v>123</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2014,12 +2111,20 @@
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+    <row r="38" ht="37.5" customHeight="1">
+      <c r="A38" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="5"/>
+      <c r="E38" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -7091,2444 +7196,2337 @@
       <c r="Y225" s="3"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="3"/>
-      <c r="B226" s="5"/>
-      <c r="C226" s="5"/>
-      <c r="D226" s="3"/>
-      <c r="E226" s="5"/>
-      <c r="F226" s="3"/>
-      <c r="G226" s="3"/>
-      <c r="H226" s="3"/>
-      <c r="I226" s="3"/>
-      <c r="J226" s="3"/>
-      <c r="K226" s="3"/>
-      <c r="L226" s="3"/>
-      <c r="M226" s="3"/>
-      <c r="N226" s="3"/>
-      <c r="O226" s="3"/>
-      <c r="P226" s="3"/>
-      <c r="Q226" s="3"/>
-      <c r="R226" s="3"/>
-      <c r="S226" s="3"/>
-      <c r="T226" s="3"/>
-      <c r="U226" s="3"/>
-      <c r="V226" s="3"/>
-      <c r="W226" s="3"/>
-      <c r="X226" s="3"/>
-      <c r="Y226" s="3"/>
+      <c r="B226" s="16"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="3"/>
-      <c r="B227" s="5"/>
-      <c r="C227" s="5"/>
-      <c r="D227" s="3"/>
-      <c r="E227" s="5"/>
-      <c r="F227" s="3"/>
-      <c r="G227" s="3"/>
-      <c r="H227" s="3"/>
-      <c r="I227" s="3"/>
-      <c r="J227" s="3"/>
-      <c r="K227" s="3"/>
-      <c r="L227" s="3"/>
-      <c r="M227" s="3"/>
-      <c r="N227" s="3"/>
-      <c r="O227" s="3"/>
-      <c r="P227" s="3"/>
-      <c r="Q227" s="3"/>
-      <c r="R227" s="3"/>
-      <c r="S227" s="3"/>
-      <c r="T227" s="3"/>
-      <c r="U227" s="3"/>
-      <c r="V227" s="3"/>
-      <c r="W227" s="3"/>
-      <c r="X227" s="3"/>
-      <c r="Y227" s="3"/>
+      <c r="B227" s="16"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="3"/>
-      <c r="B228" s="5"/>
-      <c r="C228" s="5"/>
-      <c r="D228" s="3"/>
-      <c r="E228" s="5"/>
-      <c r="F228" s="3"/>
-      <c r="G228" s="3"/>
-      <c r="H228" s="3"/>
-      <c r="I228" s="3"/>
-      <c r="J228" s="3"/>
-      <c r="K228" s="3"/>
-      <c r="L228" s="3"/>
-      <c r="M228" s="3"/>
-      <c r="N228" s="3"/>
-      <c r="O228" s="3"/>
-      <c r="P228" s="3"/>
-      <c r="Q228" s="3"/>
-      <c r="R228" s="3"/>
-      <c r="S228" s="3"/>
-      <c r="T228" s="3"/>
-      <c r="U228" s="3"/>
-      <c r="V228" s="3"/>
-      <c r="W228" s="3"/>
-      <c r="X228" s="3"/>
-      <c r="Y228" s="3"/>
+      <c r="B228" s="16"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="3"/>
-      <c r="B229" s="5"/>
-      <c r="C229" s="5"/>
-      <c r="D229" s="3"/>
-      <c r="E229" s="5"/>
-      <c r="F229" s="3"/>
-      <c r="G229" s="3"/>
-      <c r="H229" s="3"/>
-      <c r="I229" s="3"/>
-      <c r="J229" s="3"/>
-      <c r="K229" s="3"/>
-      <c r="L229" s="3"/>
-      <c r="M229" s="3"/>
-      <c r="N229" s="3"/>
-      <c r="O229" s="3"/>
-      <c r="P229" s="3"/>
-      <c r="Q229" s="3"/>
-      <c r="R229" s="3"/>
-      <c r="S229" s="3"/>
-      <c r="T229" s="3"/>
-      <c r="U229" s="3"/>
-      <c r="V229" s="3"/>
-      <c r="W229" s="3"/>
-      <c r="X229" s="3"/>
-      <c r="Y229" s="3"/>
+      <c r="B229" s="16"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="B230" s="13"/>
+      <c r="B230" s="16"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="B231" s="13"/>
+      <c r="B231" s="16"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="B232" s="13"/>
+      <c r="B232" s="16"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="B233" s="13"/>
+      <c r="B233" s="16"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="B234" s="13"/>
+      <c r="B234" s="16"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="B235" s="13"/>
+      <c r="B235" s="16"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="B236" s="13"/>
+      <c r="B236" s="16"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="B237" s="13"/>
+      <c r="B237" s="16"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="B238" s="13"/>
+      <c r="B238" s="16"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="B239" s="13"/>
+      <c r="B239" s="16"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="B240" s="13"/>
+      <c r="B240" s="16"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="B241" s="13"/>
+      <c r="B241" s="16"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="B242" s="13"/>
+      <c r="B242" s="16"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="B243" s="13"/>
+      <c r="B243" s="16"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="B244" s="13"/>
+      <c r="B244" s="16"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="B245" s="13"/>
+      <c r="B245" s="16"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="B246" s="13"/>
+      <c r="B246" s="16"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="B247" s="13"/>
+      <c r="B247" s="16"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="B248" s="13"/>
+      <c r="B248" s="16"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="B249" s="13"/>
+      <c r="B249" s="16"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="B250" s="13"/>
+      <c r="B250" s="16"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="B251" s="13"/>
+      <c r="B251" s="16"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="B252" s="13"/>
+      <c r="B252" s="16"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="B253" s="13"/>
+      <c r="B253" s="16"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="B254" s="13"/>
+      <c r="B254" s="16"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="B255" s="13"/>
+      <c r="B255" s="16"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="B256" s="13"/>
+      <c r="B256" s="16"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="B257" s="13"/>
+      <c r="B257" s="16"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="B258" s="13"/>
+      <c r="B258" s="16"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="13"/>
+      <c r="B259" s="16"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="B260" s="13"/>
+      <c r="B260" s="16"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="B261" s="13"/>
+      <c r="B261" s="16"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="B262" s="13"/>
+      <c r="B262" s="16"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="B263" s="13"/>
+      <c r="B263" s="16"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="B264" s="13"/>
+      <c r="B264" s="16"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="B265" s="13"/>
+      <c r="B265" s="16"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="B266" s="13"/>
+      <c r="B266" s="16"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="B267" s="13"/>
+      <c r="B267" s="16"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="B268" s="13"/>
+      <c r="B268" s="16"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="B269" s="13"/>
+      <c r="B269" s="16"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="B270" s="13"/>
+      <c r="B270" s="16"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="B271" s="13"/>
+      <c r="B271" s="16"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="B272" s="13"/>
+      <c r="B272" s="16"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="B273" s="13"/>
+      <c r="B273" s="16"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="B274" s="13"/>
+      <c r="B274" s="16"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="B275" s="13"/>
+      <c r="B275" s="16"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="B276" s="13"/>
+      <c r="B276" s="16"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="B277" s="13"/>
+      <c r="B277" s="16"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="B278" s="13"/>
+      <c r="B278" s="16"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="B279" s="13"/>
+      <c r="B279" s="16"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="B280" s="13"/>
+      <c r="B280" s="16"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="B281" s="13"/>
+      <c r="B281" s="16"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="B282" s="13"/>
+      <c r="B282" s="16"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="B283" s="13"/>
+      <c r="B283" s="16"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="B284" s="13"/>
+      <c r="B284" s="16"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="B285" s="13"/>
+      <c r="B285" s="16"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="B286" s="13"/>
+      <c r="B286" s="16"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="B287" s="13"/>
+      <c r="B287" s="16"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="B288" s="13"/>
+      <c r="B288" s="16"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="B289" s="13"/>
+      <c r="B289" s="16"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="B290" s="13"/>
+      <c r="B290" s="16"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="B291" s="13"/>
+      <c r="B291" s="16"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="B292" s="13"/>
+      <c r="B292" s="16"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="B293" s="13"/>
+      <c r="B293" s="16"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="B294" s="13"/>
+      <c r="B294" s="16"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="B295" s="13"/>
+      <c r="B295" s="16"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="B296" s="13"/>
+      <c r="B296" s="16"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="B297" s="13"/>
+      <c r="B297" s="16"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="B298" s="13"/>
+      <c r="B298" s="16"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="B299" s="13"/>
+      <c r="B299" s="16"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="B300" s="13"/>
+      <c r="B300" s="16"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="B301" s="13"/>
+      <c r="B301" s="16"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="B302" s="13"/>
+      <c r="B302" s="16"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="B303" s="13"/>
+      <c r="B303" s="16"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="B304" s="13"/>
+      <c r="B304" s="16"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="B305" s="13"/>
+      <c r="B305" s="16"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="B306" s="13"/>
+      <c r="B306" s="16"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="B307" s="13"/>
+      <c r="B307" s="16"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="B308" s="13"/>
+      <c r="B308" s="16"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="B309" s="13"/>
+      <c r="B309" s="16"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="B310" s="13"/>
+      <c r="B310" s="16"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="B311" s="13"/>
+      <c r="B311" s="16"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="B312" s="13"/>
+      <c r="B312" s="16"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="B313" s="13"/>
+      <c r="B313" s="16"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="B314" s="13"/>
+      <c r="B314" s="16"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="B315" s="13"/>
+      <c r="B315" s="16"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="B316" s="13"/>
+      <c r="B316" s="16"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="B317" s="13"/>
+      <c r="B317" s="16"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="B318" s="13"/>
+      <c r="B318" s="16"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="B319" s="13"/>
+      <c r="B319" s="16"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="B320" s="13"/>
+      <c r="B320" s="16"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="B321" s="13"/>
+      <c r="B321" s="16"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="B322" s="13"/>
+      <c r="B322" s="16"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="B323" s="13"/>
+      <c r="B323" s="16"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="B324" s="13"/>
+      <c r="B324" s="16"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="B325" s="13"/>
+      <c r="B325" s="16"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="B326" s="13"/>
+      <c r="B326" s="16"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="B327" s="13"/>
+      <c r="B327" s="16"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="B328" s="13"/>
+      <c r="B328" s="16"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="B329" s="13"/>
+      <c r="B329" s="16"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="B330" s="13"/>
+      <c r="B330" s="16"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="B331" s="13"/>
+      <c r="B331" s="16"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="B332" s="13"/>
+      <c r="B332" s="16"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="B333" s="13"/>
+      <c r="B333" s="16"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="B334" s="13"/>
+      <c r="B334" s="16"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="B335" s="13"/>
+      <c r="B335" s="16"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="B336" s="13"/>
+      <c r="B336" s="16"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="B337" s="13"/>
+      <c r="B337" s="16"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="B338" s="13"/>
+      <c r="B338" s="16"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="B339" s="13"/>
+      <c r="B339" s="16"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="B340" s="13"/>
+      <c r="B340" s="16"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="B341" s="13"/>
+      <c r="B341" s="16"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="B342" s="13"/>
+      <c r="B342" s="16"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="B343" s="13"/>
+      <c r="B343" s="16"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="B344" s="13"/>
+      <c r="B344" s="16"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="B345" s="13"/>
+      <c r="B345" s="16"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="B346" s="13"/>
+      <c r="B346" s="16"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="B347" s="13"/>
+      <c r="B347" s="16"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="B348" s="13"/>
+      <c r="B348" s="16"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="B349" s="13"/>
+      <c r="B349" s="16"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="B350" s="13"/>
+      <c r="B350" s="16"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="B351" s="13"/>
+      <c r="B351" s="16"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="B352" s="13"/>
+      <c r="B352" s="16"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="B353" s="13"/>
+      <c r="B353" s="16"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="B354" s="13"/>
+      <c r="B354" s="16"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="B355" s="13"/>
+      <c r="B355" s="16"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="B356" s="13"/>
+      <c r="B356" s="16"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="B357" s="13"/>
+      <c r="B357" s="16"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="B358" s="13"/>
+      <c r="B358" s="16"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="B359" s="13"/>
+      <c r="B359" s="16"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="B360" s="13"/>
+      <c r="B360" s="16"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="B361" s="13"/>
+      <c r="B361" s="16"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="B362" s="13"/>
+      <c r="B362" s="16"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="B363" s="13"/>
+      <c r="B363" s="16"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="B364" s="13"/>
+      <c r="B364" s="16"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="B365" s="13"/>
+      <c r="B365" s="16"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="B366" s="13"/>
+      <c r="B366" s="16"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="B367" s="13"/>
+      <c r="B367" s="16"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="B368" s="13"/>
+      <c r="B368" s="16"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="B369" s="13"/>
+      <c r="B369" s="16"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="B370" s="13"/>
+      <c r="B370" s="16"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="B371" s="13"/>
+      <c r="B371" s="16"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="B372" s="13"/>
+      <c r="B372" s="16"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="B373" s="13"/>
+      <c r="B373" s="16"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="B374" s="13"/>
+      <c r="B374" s="16"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="B375" s="13"/>
+      <c r="B375" s="16"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="B376" s="13"/>
+      <c r="B376" s="16"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="B377" s="13"/>
+      <c r="B377" s="16"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="B378" s="13"/>
+      <c r="B378" s="16"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="13"/>
+      <c r="B379" s="16"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="B380" s="13"/>
+      <c r="B380" s="16"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="B381" s="13"/>
+      <c r="B381" s="16"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="B382" s="13"/>
+      <c r="B382" s="16"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="B383" s="13"/>
+      <c r="B383" s="16"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="B384" s="13"/>
+      <c r="B384" s="16"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="B385" s="13"/>
+      <c r="B385" s="16"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="B386" s="13"/>
+      <c r="B386" s="16"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="B387" s="13"/>
+      <c r="B387" s="16"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="B388" s="13"/>
+      <c r="B388" s="16"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="B389" s="13"/>
+      <c r="B389" s="16"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="13"/>
+      <c r="B390" s="16"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="B391" s="13"/>
+      <c r="B391" s="16"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="B392" s="13"/>
+      <c r="B392" s="16"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="B393" s="13"/>
+      <c r="B393" s="16"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="B394" s="13"/>
+      <c r="B394" s="16"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="B395" s="13"/>
+      <c r="B395" s="16"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="B396" s="13"/>
+      <c r="B396" s="16"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="B397" s="13"/>
+      <c r="B397" s="16"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="B398" s="13"/>
+      <c r="B398" s="16"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="B399" s="13"/>
+      <c r="B399" s="16"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="B400" s="13"/>
+      <c r="B400" s="16"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="B401" s="13"/>
+      <c r="B401" s="16"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="B402" s="13"/>
+      <c r="B402" s="16"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="B403" s="13"/>
+      <c r="B403" s="16"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="B404" s="13"/>
+      <c r="B404" s="16"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="B405" s="13"/>
+      <c r="B405" s="16"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="B406" s="13"/>
+      <c r="B406" s="16"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="B407" s="13"/>
+      <c r="B407" s="16"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="B408" s="13"/>
+      <c r="B408" s="16"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="B409" s="13"/>
+      <c r="B409" s="16"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="B410" s="13"/>
+      <c r="B410" s="16"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="B411" s="13"/>
+      <c r="B411" s="16"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="B412" s="13"/>
+      <c r="B412" s="16"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="B413" s="13"/>
+      <c r="B413" s="16"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="B414" s="13"/>
+      <c r="B414" s="16"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="B415" s="13"/>
+      <c r="B415" s="16"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="B416" s="13"/>
+      <c r="B416" s="16"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="B417" s="13"/>
+      <c r="B417" s="16"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="B418" s="13"/>
+      <c r="B418" s="16"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="B419" s="13"/>
+      <c r="B419" s="16"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="B420" s="13"/>
+      <c r="B420" s="16"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="B421" s="13"/>
+      <c r="B421" s="16"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="B422" s="13"/>
+      <c r="B422" s="16"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="B423" s="13"/>
+      <c r="B423" s="16"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="B424" s="13"/>
+      <c r="B424" s="16"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="B425" s="13"/>
+      <c r="B425" s="16"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="B426" s="13"/>
+      <c r="B426" s="16"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="B427" s="13"/>
+      <c r="B427" s="16"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="B428" s="13"/>
+      <c r="B428" s="16"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="B429" s="13"/>
+      <c r="B429" s="16"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="B430" s="13"/>
+      <c r="B430" s="16"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="B431" s="13"/>
+      <c r="B431" s="16"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="B432" s="13"/>
+      <c r="B432" s="16"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="B433" s="13"/>
+      <c r="B433" s="16"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="B434" s="13"/>
+      <c r="B434" s="16"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="B435" s="13"/>
+      <c r="B435" s="16"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="B436" s="13"/>
+      <c r="B436" s="16"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="B437" s="13"/>
+      <c r="B437" s="16"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="B438" s="13"/>
+      <c r="B438" s="16"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="B439" s="13"/>
+      <c r="B439" s="16"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="13"/>
+      <c r="B440" s="16"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="B441" s="13"/>
+      <c r="B441" s="16"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="B442" s="13"/>
+      <c r="B442" s="16"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="B443" s="13"/>
+      <c r="B443" s="16"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="B444" s="13"/>
+      <c r="B444" s="16"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="B445" s="13"/>
+      <c r="B445" s="16"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="B446" s="13"/>
+      <c r="B446" s="16"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="B447" s="13"/>
+      <c r="B447" s="16"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="B448" s="13"/>
+      <c r="B448" s="16"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="B449" s="13"/>
+      <c r="B449" s="16"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="B450" s="13"/>
+      <c r="B450" s="16"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="B451" s="13"/>
+      <c r="B451" s="16"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="B452" s="13"/>
+      <c r="B452" s="16"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="B453" s="13"/>
+      <c r="B453" s="16"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="B454" s="13"/>
+      <c r="B454" s="16"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="B455" s="13"/>
+      <c r="B455" s="16"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="B456" s="13"/>
+      <c r="B456" s="16"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="B457" s="13"/>
+      <c r="B457" s="16"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="B458" s="13"/>
+      <c r="B458" s="16"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="B459" s="13"/>
+      <c r="B459" s="16"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="B460" s="13"/>
+      <c r="B460" s="16"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="B461" s="13"/>
+      <c r="B461" s="16"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="B462" s="13"/>
+      <c r="B462" s="16"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="B463" s="13"/>
+      <c r="B463" s="16"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="B464" s="13"/>
+      <c r="B464" s="16"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="B465" s="13"/>
+      <c r="B465" s="16"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="B466" s="13"/>
+      <c r="B466" s="16"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="B467" s="13"/>
+      <c r="B467" s="16"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="B468" s="13"/>
+      <c r="B468" s="16"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="B469" s="13"/>
+      <c r="B469" s="16"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="B470" s="13"/>
+      <c r="B470" s="16"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="B471" s="13"/>
+      <c r="B471" s="16"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="B472" s="13"/>
+      <c r="B472" s="16"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="B473" s="13"/>
+      <c r="B473" s="16"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="B474" s="13"/>
+      <c r="B474" s="16"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="B475" s="13"/>
+      <c r="B475" s="16"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="B476" s="13"/>
+      <c r="B476" s="16"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="B477" s="13"/>
+      <c r="B477" s="16"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="B478" s="13"/>
+      <c r="B478" s="16"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="B479" s="13"/>
+      <c r="B479" s="16"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="B480" s="13"/>
+      <c r="B480" s="16"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="B481" s="13"/>
+      <c r="B481" s="16"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="B482" s="13"/>
+      <c r="B482" s="16"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="B483" s="13"/>
+      <c r="B483" s="16"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="B484" s="13"/>
+      <c r="B484" s="16"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="B485" s="13"/>
+      <c r="B485" s="16"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="B486" s="13"/>
+      <c r="B486" s="16"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="B487" s="13"/>
+      <c r="B487" s="16"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="B488" s="13"/>
+      <c r="B488" s="16"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="B489" s="13"/>
+      <c r="B489" s="16"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="B490" s="13"/>
+      <c r="B490" s="16"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="B491" s="13"/>
+      <c r="B491" s="16"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="B492" s="13"/>
+      <c r="B492" s="16"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="B493" s="13"/>
+      <c r="B493" s="16"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="B494" s="13"/>
+      <c r="B494" s="16"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="B495" s="13"/>
+      <c r="B495" s="16"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="B496" s="13"/>
+      <c r="B496" s="16"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="B497" s="13"/>
+      <c r="B497" s="16"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="B498" s="13"/>
+      <c r="B498" s="16"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="B499" s="13"/>
+      <c r="B499" s="16"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="B500" s="13"/>
+      <c r="B500" s="16"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="B501" s="13"/>
+      <c r="B501" s="16"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="B502" s="13"/>
+      <c r="B502" s="16"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="B503" s="13"/>
+      <c r="B503" s="16"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="B504" s="13"/>
+      <c r="B504" s="16"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="B505" s="13"/>
+      <c r="B505" s="16"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="B506" s="13"/>
+      <c r="B506" s="16"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="B507" s="13"/>
+      <c r="B507" s="16"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="B508" s="13"/>
+      <c r="B508" s="16"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="B509" s="13"/>
+      <c r="B509" s="16"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="B510" s="13"/>
+      <c r="B510" s="16"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="B511" s="13"/>
+      <c r="B511" s="16"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="B512" s="13"/>
+      <c r="B512" s="16"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="B513" s="13"/>
+      <c r="B513" s="16"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="B514" s="13"/>
+      <c r="B514" s="16"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="B515" s="13"/>
+      <c r="B515" s="16"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="B516" s="13"/>
+      <c r="B516" s="16"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="B517" s="13"/>
+      <c r="B517" s="16"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="B518" s="13"/>
+      <c r="B518" s="16"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="B519" s="13"/>
+      <c r="B519" s="16"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="B520" s="13"/>
+      <c r="B520" s="16"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="B521" s="13"/>
+      <c r="B521" s="16"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="B522" s="13"/>
+      <c r="B522" s="16"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="B523" s="13"/>
+      <c r="B523" s="16"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="B524" s="13"/>
+      <c r="B524" s="16"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="B525" s="13"/>
+      <c r="B525" s="16"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="B526" s="13"/>
+      <c r="B526" s="16"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="B527" s="13"/>
+      <c r="B527" s="16"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="B528" s="13"/>
+      <c r="B528" s="16"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="B529" s="13"/>
+      <c r="B529" s="16"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="B530" s="13"/>
+      <c r="B530" s="16"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="B531" s="13"/>
+      <c r="B531" s="16"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="B532" s="13"/>
+      <c r="B532" s="16"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="B533" s="13"/>
+      <c r="B533" s="16"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="B534" s="13"/>
+      <c r="B534" s="16"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="B535" s="13"/>
+      <c r="B535" s="16"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="B536" s="13"/>
+      <c r="B536" s="16"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="B537" s="13"/>
+      <c r="B537" s="16"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="B538" s="13"/>
+      <c r="B538" s="16"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="B539" s="13"/>
+      <c r="B539" s="16"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="B540" s="13"/>
+      <c r="B540" s="16"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="B541" s="13"/>
+      <c r="B541" s="16"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="B542" s="13"/>
+      <c r="B542" s="16"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="B543" s="13"/>
+      <c r="B543" s="16"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="B544" s="13"/>
+      <c r="B544" s="16"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="B545" s="13"/>
+      <c r="B545" s="16"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="B546" s="13"/>
+      <c r="B546" s="16"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="B547" s="13"/>
+      <c r="B547" s="16"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="B548" s="13"/>
+      <c r="B548" s="16"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="B549" s="13"/>
+      <c r="B549" s="16"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="B550" s="13"/>
+      <c r="B550" s="16"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="B551" s="13"/>
+      <c r="B551" s="16"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="B552" s="13"/>
+      <c r="B552" s="16"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="B553" s="13"/>
+      <c r="B553" s="16"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="B554" s="13"/>
+      <c r="B554" s="16"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="B555" s="13"/>
+      <c r="B555" s="16"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="B556" s="13"/>
+      <c r="B556" s="16"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="B557" s="13"/>
+      <c r="B557" s="16"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="B558" s="13"/>
+      <c r="B558" s="16"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="B559" s="13"/>
+      <c r="B559" s="16"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="B560" s="13"/>
+      <c r="B560" s="16"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="B561" s="13"/>
+      <c r="B561" s="16"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="B562" s="13"/>
+      <c r="B562" s="16"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="B563" s="13"/>
+      <c r="B563" s="16"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="B564" s="13"/>
+      <c r="B564" s="16"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="B565" s="13"/>
+      <c r="B565" s="16"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="B566" s="13"/>
+      <c r="B566" s="16"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="B567" s="13"/>
+      <c r="B567" s="16"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="B568" s="13"/>
+      <c r="B568" s="16"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="B569" s="13"/>
+      <c r="B569" s="16"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="B570" s="13"/>
+      <c r="B570" s="16"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="B571" s="13"/>
+      <c r="B571" s="16"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="B572" s="13"/>
+      <c r="B572" s="16"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="B573" s="13"/>
+      <c r="B573" s="16"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="B574" s="13"/>
+      <c r="B574" s="16"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="B575" s="13"/>
+      <c r="B575" s="16"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="B576" s="13"/>
+      <c r="B576" s="16"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="B577" s="13"/>
+      <c r="B577" s="16"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="B578" s="13"/>
+      <c r="B578" s="16"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="B579" s="13"/>
+      <c r="B579" s="16"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="B580" s="13"/>
+      <c r="B580" s="16"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="B581" s="13"/>
+      <c r="B581" s="16"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="B582" s="13"/>
+      <c r="B582" s="16"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="B583" s="13"/>
+      <c r="B583" s="16"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="B584" s="13"/>
+      <c r="B584" s="16"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="B585" s="13"/>
+      <c r="B585" s="16"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="B586" s="13"/>
+      <c r="B586" s="16"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="B587" s="13"/>
+      <c r="B587" s="16"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="B588" s="13"/>
+      <c r="B588" s="16"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="B589" s="13"/>
+      <c r="B589" s="16"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="B590" s="13"/>
+      <c r="B590" s="16"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="B591" s="13"/>
+      <c r="B591" s="16"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="B592" s="13"/>
+      <c r="B592" s="16"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="B593" s="13"/>
+      <c r="B593" s="16"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="B594" s="13"/>
+      <c r="B594" s="16"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="B595" s="13"/>
+      <c r="B595" s="16"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="B596" s="13"/>
+      <c r="B596" s="16"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="B597" s="13"/>
+      <c r="B597" s="16"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="B598" s="13"/>
+      <c r="B598" s="16"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="B599" s="13"/>
+      <c r="B599" s="16"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="B600" s="13"/>
+      <c r="B600" s="16"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="B601" s="13"/>
+      <c r="B601" s="16"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="B602" s="13"/>
+      <c r="B602" s="16"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="B603" s="13"/>
+      <c r="B603" s="16"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="B604" s="13"/>
+      <c r="B604" s="16"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="B605" s="13"/>
+      <c r="B605" s="16"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="B606" s="13"/>
+      <c r="B606" s="16"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="B607" s="13"/>
+      <c r="B607" s="16"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="B608" s="13"/>
+      <c r="B608" s="16"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="B609" s="13"/>
+      <c r="B609" s="16"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="B610" s="13"/>
+      <c r="B610" s="16"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="B611" s="13"/>
+      <c r="B611" s="16"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="B612" s="13"/>
+      <c r="B612" s="16"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="B613" s="13"/>
+      <c r="B613" s="16"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="B614" s="13"/>
+      <c r="B614" s="16"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="B615" s="13"/>
+      <c r="B615" s="16"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="B616" s="13"/>
+      <c r="B616" s="16"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="B617" s="13"/>
+      <c r="B617" s="16"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="B618" s="13"/>
+      <c r="B618" s="16"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="B619" s="13"/>
+      <c r="B619" s="16"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="B620" s="13"/>
+      <c r="B620" s="16"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="B621" s="13"/>
+      <c r="B621" s="16"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="B622" s="13"/>
+      <c r="B622" s="16"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="B623" s="13"/>
+      <c r="B623" s="16"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="B624" s="13"/>
+      <c r="B624" s="16"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="B625" s="13"/>
+      <c r="B625" s="16"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="B626" s="13"/>
+      <c r="B626" s="16"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="B627" s="13"/>
+      <c r="B627" s="16"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="B628" s="13"/>
+      <c r="B628" s="16"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="B629" s="13"/>
+      <c r="B629" s="16"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="B630" s="13"/>
+      <c r="B630" s="16"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="B631" s="13"/>
+      <c r="B631" s="16"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="B632" s="13"/>
+      <c r="B632" s="16"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="B633" s="13"/>
+      <c r="B633" s="16"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="B634" s="13"/>
+      <c r="B634" s="16"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="B635" s="13"/>
+      <c r="B635" s="16"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="B636" s="13"/>
+      <c r="B636" s="16"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="B637" s="13"/>
+      <c r="B637" s="16"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="B638" s="13"/>
+      <c r="B638" s="16"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="B639" s="13"/>
+      <c r="B639" s="16"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="B640" s="13"/>
+      <c r="B640" s="16"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="B641" s="13"/>
+      <c r="B641" s="16"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="B642" s="13"/>
+      <c r="B642" s="16"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="B643" s="13"/>
+      <c r="B643" s="16"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="B644" s="13"/>
+      <c r="B644" s="16"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="B645" s="13"/>
+      <c r="B645" s="16"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="B646" s="13"/>
+      <c r="B646" s="16"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="B647" s="13"/>
+      <c r="B647" s="16"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="B648" s="13"/>
+      <c r="B648" s="16"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="B649" s="13"/>
+      <c r="B649" s="16"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="B650" s="13"/>
+      <c r="B650" s="16"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="B651" s="13"/>
+      <c r="B651" s="16"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="B652" s="13"/>
+      <c r="B652" s="16"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="B653" s="13"/>
+      <c r="B653" s="16"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="B654" s="13"/>
+      <c r="B654" s="16"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="B655" s="13"/>
+      <c r="B655" s="16"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="B656" s="13"/>
+      <c r="B656" s="16"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="B657" s="13"/>
+      <c r="B657" s="16"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="B658" s="13"/>
+      <c r="B658" s="16"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="B659" s="13"/>
+      <c r="B659" s="16"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="B660" s="13"/>
+      <c r="B660" s="16"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="B661" s="13"/>
+      <c r="B661" s="16"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="B662" s="13"/>
+      <c r="B662" s="16"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="B663" s="13"/>
+      <c r="B663" s="16"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="B664" s="13"/>
+      <c r="B664" s="16"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="B665" s="13"/>
+      <c r="B665" s="16"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="B666" s="13"/>
+      <c r="B666" s="16"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="B667" s="13"/>
+      <c r="B667" s="16"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="B668" s="13"/>
+      <c r="B668" s="16"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="B669" s="13"/>
+      <c r="B669" s="16"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="B670" s="13"/>
+      <c r="B670" s="16"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="B671" s="13"/>
+      <c r="B671" s="16"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="B672" s="13"/>
+      <c r="B672" s="16"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="B673" s="13"/>
+      <c r="B673" s="16"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="B674" s="13"/>
+      <c r="B674" s="16"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="B675" s="13"/>
+      <c r="B675" s="16"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="B676" s="13"/>
+      <c r="B676" s="16"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="B677" s="13"/>
+      <c r="B677" s="16"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="B678" s="13"/>
+      <c r="B678" s="16"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="B679" s="13"/>
+      <c r="B679" s="16"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="B680" s="13"/>
+      <c r="B680" s="16"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="B681" s="13"/>
+      <c r="B681" s="16"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="B682" s="13"/>
+      <c r="B682" s="16"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="B683" s="13"/>
+      <c r="B683" s="16"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="B684" s="13"/>
+      <c r="B684" s="16"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="B685" s="13"/>
+      <c r="B685" s="16"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="B686" s="13"/>
+      <c r="B686" s="16"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="B687" s="13"/>
+      <c r="B687" s="16"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="B688" s="13"/>
+      <c r="B688" s="16"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="B689" s="13"/>
+      <c r="B689" s="16"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="B690" s="13"/>
+      <c r="B690" s="16"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="B691" s="13"/>
+      <c r="B691" s="16"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="B692" s="13"/>
+      <c r="B692" s="16"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="B693" s="13"/>
+      <c r="B693" s="16"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="B694" s="13"/>
+      <c r="B694" s="16"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="B695" s="13"/>
+      <c r="B695" s="16"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="B696" s="13"/>
+      <c r="B696" s="16"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="B697" s="13"/>
+      <c r="B697" s="16"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="B698" s="13"/>
+      <c r="B698" s="16"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="B699" s="13"/>
+      <c r="B699" s="16"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="B700" s="13"/>
+      <c r="B700" s="16"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="B701" s="13"/>
+      <c r="B701" s="16"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="B702" s="13"/>
+      <c r="B702" s="16"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="B703" s="13"/>
+      <c r="B703" s="16"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="B704" s="13"/>
+      <c r="B704" s="16"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="B705" s="13"/>
+      <c r="B705" s="16"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="B706" s="13"/>
+      <c r="B706" s="16"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="B707" s="13"/>
+      <c r="B707" s="16"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="B708" s="13"/>
+      <c r="B708" s="16"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="B709" s="13"/>
+      <c r="B709" s="16"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="B710" s="13"/>
+      <c r="B710" s="16"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="B711" s="13"/>
+      <c r="B711" s="16"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="B712" s="13"/>
+      <c r="B712" s="16"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="B713" s="13"/>
+      <c r="B713" s="16"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="B714" s="13"/>
+      <c r="B714" s="16"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="B715" s="13"/>
+      <c r="B715" s="16"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="B716" s="13"/>
+      <c r="B716" s="16"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="B717" s="13"/>
+      <c r="B717" s="16"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="B718" s="13"/>
+      <c r="B718" s="16"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="B719" s="13"/>
+      <c r="B719" s="16"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="B720" s="13"/>
+      <c r="B720" s="16"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="B721" s="13"/>
+      <c r="B721" s="16"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="B722" s="13"/>
+      <c r="B722" s="16"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="B723" s="13"/>
+      <c r="B723" s="16"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="B724" s="13"/>
+      <c r="B724" s="16"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="B725" s="13"/>
+      <c r="B725" s="16"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="B726" s="13"/>
+      <c r="B726" s="16"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="B727" s="13"/>
+      <c r="B727" s="16"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="B728" s="13"/>
+      <c r="B728" s="16"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="B729" s="13"/>
+      <c r="B729" s="16"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="B730" s="13"/>
+      <c r="B730" s="16"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="B731" s="13"/>
+      <c r="B731" s="16"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="B732" s="13"/>
+      <c r="B732" s="16"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="B733" s="13"/>
+      <c r="B733" s="16"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="B734" s="13"/>
+      <c r="B734" s="16"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="B735" s="13"/>
+      <c r="B735" s="16"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="B736" s="13"/>
+      <c r="B736" s="16"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="B737" s="13"/>
+      <c r="B737" s="16"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="B738" s="13"/>
+      <c r="B738" s="16"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="B739" s="13"/>
+      <c r="B739" s="16"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="B740" s="13"/>
+      <c r="B740" s="16"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="B741" s="13"/>
+      <c r="B741" s="16"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="B742" s="13"/>
+      <c r="B742" s="16"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="B743" s="13"/>
+      <c r="B743" s="16"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="B744" s="13"/>
+      <c r="B744" s="16"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="B745" s="13"/>
+      <c r="B745" s="16"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="B746" s="13"/>
+      <c r="B746" s="16"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="B747" s="13"/>
+      <c r="B747" s="16"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="B748" s="13"/>
+      <c r="B748" s="16"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="B749" s="13"/>
+      <c r="B749" s="16"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="B750" s="13"/>
+      <c r="B750" s="16"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="B751" s="13"/>
+      <c r="B751" s="16"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="B752" s="13"/>
+      <c r="B752" s="16"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="B753" s="13"/>
+      <c r="B753" s="16"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="B754" s="13"/>
+      <c r="B754" s="16"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="B755" s="13"/>
+      <c r="B755" s="16"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="B756" s="13"/>
+      <c r="B756" s="16"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="B757" s="13"/>
+      <c r="B757" s="16"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="B758" s="13"/>
+      <c r="B758" s="16"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="B759" s="13"/>
+      <c r="B759" s="16"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="B760" s="13"/>
+      <c r="B760" s="16"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="B761" s="13"/>
+      <c r="B761" s="16"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="B762" s="13"/>
+      <c r="B762" s="16"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="B763" s="13"/>
+      <c r="B763" s="16"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="B764" s="13"/>
+      <c r="B764" s="16"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="B765" s="13"/>
+      <c r="B765" s="16"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="B766" s="13"/>
+      <c r="B766" s="16"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="B767" s="13"/>
+      <c r="B767" s="16"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="B768" s="13"/>
+      <c r="B768" s="16"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="B769" s="13"/>
+      <c r="B769" s="16"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="B770" s="13"/>
+      <c r="B770" s="16"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="B771" s="13"/>
+      <c r="B771" s="16"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="B772" s="13"/>
+      <c r="B772" s="16"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="B773" s="13"/>
+      <c r="B773" s="16"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="B774" s="13"/>
+      <c r="B774" s="16"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="B775" s="13"/>
+      <c r="B775" s="16"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="B776" s="13"/>
+      <c r="B776" s="16"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="B777" s="13"/>
+      <c r="B777" s="16"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="B778" s="13"/>
+      <c r="B778" s="16"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="B779" s="13"/>
+      <c r="B779" s="16"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="B780" s="13"/>
+      <c r="B780" s="16"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="B781" s="13"/>
+      <c r="B781" s="16"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="B782" s="13"/>
+      <c r="B782" s="16"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="B783" s="13"/>
+      <c r="B783" s="16"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="B784" s="13"/>
+      <c r="B784" s="16"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="B785" s="13"/>
+      <c r="B785" s="16"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="B786" s="13"/>
+      <c r="B786" s="16"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="B787" s="13"/>
+      <c r="B787" s="16"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="B788" s="13"/>
+      <c r="B788" s="16"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="B789" s="13"/>
+      <c r="B789" s="16"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="B790" s="13"/>
+      <c r="B790" s="16"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="B791" s="13"/>
+      <c r="B791" s="16"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="B792" s="13"/>
+      <c r="B792" s="16"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="B793" s="13"/>
+      <c r="B793" s="16"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="B794" s="13"/>
+      <c r="B794" s="16"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="B795" s="13"/>
+      <c r="B795" s="16"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="B796" s="13"/>
+      <c r="B796" s="16"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="B797" s="13"/>
+      <c r="B797" s="16"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="B798" s="13"/>
+      <c r="B798" s="16"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="B799" s="13"/>
+      <c r="B799" s="16"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="B800" s="13"/>
+      <c r="B800" s="16"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="B801" s="13"/>
+      <c r="B801" s="16"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="B802" s="13"/>
+      <c r="B802" s="16"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="B803" s="13"/>
+      <c r="B803" s="16"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="B804" s="13"/>
+      <c r="B804" s="16"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="B805" s="13"/>
+      <c r="B805" s="16"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="B806" s="13"/>
+      <c r="B806" s="16"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="B807" s="13"/>
+      <c r="B807" s="16"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="B808" s="13"/>
+      <c r="B808" s="16"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="B809" s="13"/>
+      <c r="B809" s="16"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="B810" s="13"/>
+      <c r="B810" s="16"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="B811" s="13"/>
+      <c r="B811" s="16"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="B812" s="13"/>
+      <c r="B812" s="16"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="B813" s="13"/>
+      <c r="B813" s="16"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="B814" s="13"/>
+      <c r="B814" s="16"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="B815" s="13"/>
+      <c r="B815" s="16"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="B816" s="13"/>
+      <c r="B816" s="16"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="B817" s="13"/>
+      <c r="B817" s="16"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="B818" s="13"/>
+      <c r="B818" s="16"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="B819" s="13"/>
+      <c r="B819" s="16"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="B820" s="13"/>
+      <c r="B820" s="16"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="B821" s="13"/>
+      <c r="B821" s="16"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="B822" s="13"/>
+      <c r="B822" s="16"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="B823" s="13"/>
+      <c r="B823" s="16"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="B824" s="13"/>
+      <c r="B824" s="16"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="B825" s="13"/>
+      <c r="B825" s="16"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="B826" s="13"/>
+      <c r="B826" s="16"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="B827" s="13"/>
+      <c r="B827" s="16"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="B828" s="13"/>
+      <c r="B828" s="16"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="B829" s="13"/>
+      <c r="B829" s="16"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="B830" s="13"/>
+      <c r="B830" s="16"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="B831" s="13"/>
+      <c r="B831" s="16"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="B832" s="13"/>
+      <c r="B832" s="16"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="B833" s="13"/>
+      <c r="B833" s="16"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="B834" s="13"/>
+      <c r="B834" s="16"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="B835" s="13"/>
+      <c r="B835" s="16"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="B836" s="13"/>
+      <c r="B836" s="16"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="B837" s="13"/>
+      <c r="B837" s="16"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="B838" s="13"/>
+      <c r="B838" s="16"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="B839" s="13"/>
+      <c r="B839" s="16"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="B840" s="13"/>
+      <c r="B840" s="16"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="B841" s="13"/>
+      <c r="B841" s="16"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="B842" s="13"/>
+      <c r="B842" s="16"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="B843" s="13"/>
+      <c r="B843" s="16"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="B844" s="13"/>
+      <c r="B844" s="16"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="B845" s="13"/>
+      <c r="B845" s="16"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="B846" s="13"/>
+      <c r="B846" s="16"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="B847" s="13"/>
+      <c r="B847" s="16"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="B848" s="13"/>
+      <c r="B848" s="16"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="B849" s="13"/>
+      <c r="B849" s="16"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="B850" s="13"/>
+      <c r="B850" s="16"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="B851" s="13"/>
+      <c r="B851" s="16"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="B852" s="13"/>
+      <c r="B852" s="16"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="B853" s="13"/>
+      <c r="B853" s="16"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="B854" s="13"/>
+      <c r="B854" s="16"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="B855" s="13"/>
+      <c r="B855" s="16"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="B856" s="13"/>
+      <c r="B856" s="16"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="B857" s="13"/>
+      <c r="B857" s="16"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="B858" s="13"/>
+      <c r="B858" s="16"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="B859" s="13"/>
+      <c r="B859" s="16"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="B860" s="13"/>
+      <c r="B860" s="16"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="B861" s="13"/>
+      <c r="B861" s="16"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="B862" s="13"/>
+      <c r="B862" s="16"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="B863" s="13"/>
+      <c r="B863" s="16"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="B864" s="13"/>
+      <c r="B864" s="16"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="B865" s="13"/>
+      <c r="B865" s="16"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="B866" s="13"/>
+      <c r="B866" s="16"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="B867" s="13"/>
+      <c r="B867" s="16"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="B868" s="13"/>
+      <c r="B868" s="16"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="B869" s="13"/>
+      <c r="B869" s="16"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="B870" s="13"/>
+      <c r="B870" s="16"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="B871" s="13"/>
+      <c r="B871" s="16"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="B872" s="13"/>
+      <c r="B872" s="16"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="B873" s="13"/>
+      <c r="B873" s="16"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="B874" s="13"/>
+      <c r="B874" s="16"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="B875" s="13"/>
+      <c r="B875" s="16"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="B876" s="13"/>
+      <c r="B876" s="16"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="B877" s="13"/>
+      <c r="B877" s="16"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="B878" s="13"/>
+      <c r="B878" s="16"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="B879" s="13"/>
+      <c r="B879" s="16"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="B880" s="13"/>
+      <c r="B880" s="16"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="B881" s="13"/>
+      <c r="B881" s="16"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="B882" s="13"/>
+      <c r="B882" s="16"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="B883" s="13"/>
+      <c r="B883" s="16"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="B884" s="13"/>
+      <c r="B884" s="16"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="B885" s="13"/>
+      <c r="B885" s="16"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="B886" s="13"/>
+      <c r="B886" s="16"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="B887" s="13"/>
+      <c r="B887" s="16"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="B888" s="13"/>
+      <c r="B888" s="16"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="B889" s="13"/>
+      <c r="B889" s="16"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="B890" s="13"/>
+      <c r="B890" s="16"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="B891" s="13"/>
+      <c r="B891" s="16"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="B892" s="13"/>
+      <c r="B892" s="16"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="B893" s="13"/>
+      <c r="B893" s="16"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="B894" s="13"/>
+      <c r="B894" s="16"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="B895" s="13"/>
+      <c r="B895" s="16"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="B896" s="13"/>
+      <c r="B896" s="16"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="B897" s="13"/>
+      <c r="B897" s="16"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="B898" s="13"/>
+      <c r="B898" s="16"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="B899" s="13"/>
+      <c r="B899" s="16"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="B900" s="13"/>
+      <c r="B900" s="16"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="B901" s="13"/>
+      <c r="B901" s="16"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="B902" s="13"/>
+      <c r="B902" s="16"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="B903" s="13"/>
+      <c r="B903" s="16"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="B904" s="13"/>
+      <c r="B904" s="16"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="B905" s="13"/>
+      <c r="B905" s="16"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="B906" s="13"/>
+      <c r="B906" s="16"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="B907" s="13"/>
+      <c r="B907" s="16"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="B908" s="13"/>
+      <c r="B908" s="16"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="B909" s="13"/>
+      <c r="B909" s="16"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="B910" s="13"/>
+      <c r="B910" s="16"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="B911" s="13"/>
+      <c r="B911" s="16"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="B912" s="13"/>
+      <c r="B912" s="16"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="B913" s="13"/>
+      <c r="B913" s="16"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="B914" s="13"/>
+      <c r="B914" s="16"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="B915" s="13"/>
+      <c r="B915" s="16"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="B916" s="13"/>
+      <c r="B916" s="16"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="B917" s="13"/>
+      <c r="B917" s="16"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="B918" s="13"/>
+      <c r="B918" s="16"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="B919" s="13"/>
+      <c r="B919" s="16"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="B920" s="13"/>
+      <c r="B920" s="16"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="B921" s="13"/>
+      <c r="B921" s="16"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="B922" s="13"/>
+      <c r="B922" s="16"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="B923" s="13"/>
+      <c r="B923" s="16"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="B924" s="13"/>
+      <c r="B924" s="16"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="B925" s="13"/>
+      <c r="B925" s="16"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="B926" s="13"/>
+      <c r="B926" s="16"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="B927" s="13"/>
+      <c r="B927" s="16"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="B928" s="13"/>
+      <c r="B928" s="16"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="B929" s="13"/>
+      <c r="B929" s="16"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="B930" s="13"/>
+      <c r="B930" s="16"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="B931" s="13"/>
+      <c r="B931" s="16"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="B932" s="13"/>
+      <c r="B932" s="16"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="B933" s="13"/>
+      <c r="B933" s="16"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="B934" s="13"/>
+      <c r="B934" s="16"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="B935" s="13"/>
+      <c r="B935" s="16"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="B936" s="13"/>
+      <c r="B936" s="16"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="B937" s="13"/>
+      <c r="B937" s="16"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="B938" s="13"/>
+      <c r="B938" s="16"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="B939" s="13"/>
+      <c r="B939" s="16"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="B940" s="13"/>
+      <c r="B940" s="16"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="B941" s="13"/>
+      <c r="B941" s="16"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="B942" s="13"/>
+      <c r="B942" s="16"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="B943" s="13"/>
+      <c r="B943" s="16"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="B944" s="13"/>
+      <c r="B944" s="16"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="B945" s="13"/>
+      <c r="B945" s="16"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="B946" s="13"/>
+      <c r="B946" s="16"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="B947" s="13"/>
+      <c r="B947" s="16"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="B948" s="13"/>
+      <c r="B948" s="16"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="B949" s="13"/>
+      <c r="B949" s="16"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="B950" s="13"/>
+      <c r="B950" s="16"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="B951" s="13"/>
+      <c r="B951" s="16"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="B952" s="13"/>
+      <c r="B952" s="16"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="B953" s="13"/>
+      <c r="B953" s="16"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="B954" s="13"/>
+      <c r="B954" s="16"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="B955" s="13"/>
+      <c r="B955" s="16"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="B956" s="13"/>
+      <c r="B956" s="16"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="B957" s="13"/>
+      <c r="B957" s="16"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="B958" s="13"/>
+      <c r="B958" s="16"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="B959" s="13"/>
+      <c r="B959" s="16"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="B960" s="13"/>
+      <c r="B960" s="16"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="B961" s="13"/>
+      <c r="B961" s="16"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="B962" s="13"/>
+      <c r="B962" s="16"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="B963" s="13"/>
+      <c r="B963" s="16"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="B964" s="13"/>
+      <c r="B964" s="16"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="B965" s="13"/>
+      <c r="B965" s="16"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="B966" s="13"/>
+      <c r="B966" s="16"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="B967" s="13"/>
+      <c r="B967" s="16"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="B968" s="13"/>
+      <c r="B968" s="16"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="B969" s="13"/>
+      <c r="B969" s="16"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="B970" s="13"/>
+      <c r="B970" s="16"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="B971" s="13"/>
+      <c r="B971" s="16"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="B972" s="13"/>
+      <c r="B972" s="16"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="B973" s="13"/>
+      <c r="B973" s="16"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="B974" s="13"/>
+      <c r="B974" s="16"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="B975" s="13"/>
+      <c r="B975" s="16"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="B976" s="13"/>
+      <c r="B976" s="16"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="B977" s="13"/>
+      <c r="B977" s="16"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="B978" s="13"/>
+      <c r="B978" s="16"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="B979" s="13"/>
+      <c r="B979" s="16"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="B980" s="13"/>
+      <c r="B980" s="16"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="B981" s="13"/>
+      <c r="B981" s="16"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="B982" s="13"/>
+      <c r="B982" s="16"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="B983" s="13"/>
+      <c r="B983" s="16"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="B984" s="13"/>
+      <c r="B984" s="16"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="B985" s="13"/>
+      <c r="B985" s="16"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="B986" s="13"/>
+      <c r="B986" s="16"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="B987" s="13"/>
+      <c r="B987" s="16"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="B988" s="13"/>
+      <c r="B988" s="16"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="B989" s="13"/>
+      <c r="B989" s="16"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="B990" s="13"/>
+      <c r="B990" s="16"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="B991" s="13"/>
+      <c r="B991" s="16"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="B992" s="13"/>
+      <c r="B992" s="16"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="B993" s="13"/>
+      <c r="B993" s="16"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="B994" s="13"/>
+      <c r="B994" s="16"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
-      <c r="B995" s="13"/>
+      <c r="B995" s="16"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
-      <c r="B996" s="13"/>
+      <c r="B996" s="16"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
-      <c r="B997" s="13"/>
+      <c r="B997" s="16"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
-      <c r="B998" s="13"/>
+      <c r="B998" s="16"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
-      <c r="B999" s="13"/>
-    </row>
-    <row r="1000" ht="15.75" customHeight="1">
-      <c r="B1000" s="13"/>
-    </row>
-    <row r="1001" ht="15.75" customHeight="1">
-      <c r="B1001" s="13"/>
-    </row>
-    <row r="1002" ht="15.75" customHeight="1">
-      <c r="B1002" s="13"/>
-    </row>
-    <row r="1003" ht="15.75" customHeight="1">
-      <c r="B1003" s="13"/>
+      <c r="B999" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A35:E35"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new testcases for User Login
</commit_message>
<xml_diff>
--- a/TestCases_of_Idx-Auto-Tester.xlsx
+++ b/TestCases_of_Idx-Auto-Tester.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritiksh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritiksh/Desktop/idx-auto-tester/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37590449-1AF3-6C42-8320-F51C123A0A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22BAF0E-7768-544C-AD28-FED66106C9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9550F3D5-A8D2-EA40-95F3-69C57A51D18A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{9550F3D5-A8D2-EA40-95F3-69C57A51D18A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="142">
   <si>
     <t>Test case ID</t>
   </si>
@@ -617,6 +617,27 @@
   </si>
   <si>
     <t>TC_31</t>
+  </si>
+  <si>
+    <t>Verify that it should show validation message when enter email field left blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to Site URL
+2. Navigate to Login Page
+3. Leave Email Id blank and enter random Password
+4. Click on Login button </t>
+  </si>
+  <si>
+    <t>Verify that it should show validation message when enter password field left blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to Site URL
+2. Navigate to Login Page
+3. Enter Email Id  and leave Password blank
+4. Click on Login button </t>
+  </si>
+  <si>
+    <t>A validation message should show under the password input field</t>
   </si>
 </sst>
 </file>
@@ -636,21 +657,25 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF032F62"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -710,16 +735,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -736,9 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -763,6 +782,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1078,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D91CF45-591A-F240-8555-244BE922987C}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1119,7 @@
     <col min="5" max="5" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,563 +1136,594 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="56" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="84" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:6" ht="84" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="56" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="12" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="13" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+    <row r="14" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="126" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+    <row r="15" spans="1:6" ht="126" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="84" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:6" ht="84" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="84" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:5" ht="84" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="18" spans="1:5" ht="70" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+    <row r="19" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B20" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+    <row r="21" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+    <row r="22" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="126" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" ht="126" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="126" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+    <row r="24" spans="1:5" ht="126" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C24" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="140" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+    <row r="25" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="12" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="140" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="26" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="12" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="140" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+    <row r="27" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="12" t="s">
+      <c r="D27" s="12"/>
+      <c r="E27" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+    <row r="28" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="140" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+    </row>
+    <row r="29" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="126" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+    <row r="30" spans="1:5" ht="126" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+    <row r="31" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" ht="196" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+    </row>
+    <row r="32" spans="1:5" ht="196" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+    <row r="33" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" ht="126" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" ht="126" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B34" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C34" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17" t="s">
+      <c r="D34" s="14"/>
+      <c r="E34" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+    <row r="35" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B35" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C35" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17" t="s">
+      <c r="D35" s="14"/>
+      <c r="E35" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+    <row r="36" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" ht="98" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37" spans="1:5" ht="98" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+    <row r="38" spans="1:5" ht="70" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C38" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="18" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="56" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
+    <row r="39" spans="1:5" ht="56" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B39" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="18" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+    <row r="40" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" ht="196" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" spans="1:5" ht="196" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="12" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="168" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
+    <row r="42" spans="1:5" ht="168" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12" t="s">
+      <c r="D42" s="9"/>
+      <c r="E42" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="84" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
+    <row r="43" spans="1:5" ht="84" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B43" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C43" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12" t="s">
+      <c r="D43" s="9"/>
+      <c r="E43" s="10" t="s">
         <v>134</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A40:E40"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>